<commit_message>
updated URL for Aseul
</commit_message>
<xml_diff>
--- a/NewYorkTimes2020GlobalPlaylist.xlsx
+++ b/NewYorkTimes2020GlobalPlaylist.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agrogan\Box Sync\Box Sync\GitHub\research\NYTimes2020GlobalPlaylist\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agrogan\Box Sync\Box Sync\GitHub\playlist\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -189,28 +189,23 @@
     <t>Aseul</t>
   </si>
   <si>
-    <t>https://youtu.be/4Ti34K4OhCY</t>
+    <t>https://youtu.be/Vs-J3-1YQ-I</t>
   </si>
   <si>
     <t>South Korea</t>
   </si>
   <si>
-    <t>&lt;iframe width="560" height="315" src="https://www.youtube.com/embed/4Ti34K4OhCY" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture" allowfullscreen&gt;&lt;/iframe&gt;</t>
+    <t>&lt;iframe width="560" height="315" src="https://www.youtube.com/embed/Vs-J3-1YQ-I" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture" allowfullscreen&gt;&lt;/iframe&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -225,13 +220,13 @@
       <name val="Arial"/>
     </font>
     <font>
+      <u/>
       <sz val="10"/>
+      <color rgb="FF1155CC"/>
       <name val="Arial"/>
     </font>
     <font>
-      <u/>
       <sz val="10"/>
-      <color rgb="FF1155CC"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -255,13 +250,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -512,135 +506,135 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="2" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="2" t="s">
         <v>42</v>
       </c>
       <c r="G8" s="4" t="s">
@@ -648,16 +642,16 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="2" t="s">
         <v>47</v>
       </c>
       <c r="G9" s="4" t="s">
@@ -665,16 +659,16 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="2" t="s">
         <v>52</v>
       </c>
       <c r="G10" s="4" t="s">
@@ -682,16 +676,16 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>57</v>
       </c>
       <c r="G11" s="4" t="s">

</xml_diff>